<commit_message>
added 141 160 647 739
</commit_message>
<xml_diff>
--- a/record.xlsx
+++ b/record.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cufew\Desktop\leetcode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\lc_solutions\Leetcode_solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CF51B0-A5D2-4A6A-81BE-4585C90BB512}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64226844-173C-48A7-925C-F2CF523BE507}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E829B4E1-069F-413C-9F00-1850C6F04BEF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E829B4E1-069F-413C-9F00-1850C6F04BEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -763,6 +757,25 @@
   </si>
   <si>
     <t>否（有hint）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Find the Difference</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Easy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Given two strings s and t which consist of only lowercase letters.
+String t is generated by random shuffling string s and then add one more letter at a random position.
+Find the letter that was added in t.</t>
+  </si>
+  <si>
+    <t>1.HashMap
+2.Sorting
+3.XOR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1230,20 +1243,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6BDA83-FDB5-4B0C-985C-274D27E56327}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64.08203125" customWidth="1"/>
+    <col min="5" max="5" width="64.125" customWidth="1"/>
     <col min="7" max="7" width="63.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1269,7 +1282,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>43897</v>
       </c>
@@ -1295,7 +1308,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>43897</v>
       </c>
@@ -1321,7 +1334,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="94" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="93.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -1347,7 +1360,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>43897</v>
       </c>
@@ -1373,7 +1386,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>43897</v>
       </c>
@@ -1399,7 +1412,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>43897</v>
       </c>
@@ -1425,7 +1438,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43874</v>
       </c>
@@ -1451,7 +1464,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43897</v>
       </c>
@@ -1477,7 +1490,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="70" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43898</v>
       </c>
@@ -1503,7 +1516,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="84" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43911</v>
       </c>
@@ -1529,7 +1542,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="84" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43911</v>
       </c>
@@ -1555,7 +1568,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="63" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="63" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43911</v>
       </c>
@@ -1581,7 +1594,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43918</v>
       </c>
@@ -1607,7 +1620,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43918</v>
       </c>
@@ -1633,7 +1646,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="98" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43923</v>
       </c>
@@ -1659,7 +1672,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43924</v>
       </c>
@@ -1685,7 +1698,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43925</v>
       </c>
@@ -1711,7 +1724,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="126" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43926</v>
       </c>
@@ -1737,7 +1750,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43926</v>
       </c>
@@ -1763,7 +1776,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43927</v>
       </c>
@@ -1789,7 +1802,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43930</v>
       </c>
@@ -1815,7 +1828,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="98" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43931</v>
       </c>
@@ -1841,7 +1854,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43932</v>
       </c>
@@ -1865,6 +1878,29 @@
       </c>
       <c r="H24" s="2" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>44098</v>
+      </c>
+      <c r="B25" s="2">
+        <v>389</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>